<commit_message>
Changing Text Case (UPPER, LOWER, PROPER)
</commit_message>
<xml_diff>
--- a/Intermediate I/Week 2/workbook/W2_V2 Changing_Case.xlsx
+++ b/Intermediate I/Week 2/workbook/W2_V2 Changing_Case.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users-Data\mq20021873\Desktop\Coursera 20 April 2017\Course 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\foongmin\Desktop\excel-skills-for-business\Intermediate I\Week 2\workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EE7D6E-0249-40B6-AAA4-067135E775C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672"/>
+    <workbookView xWindow="9580" yWindow="0" windowWidth="9620" windowHeight="5110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$J$24</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -512,7 +521,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -933,31 +942,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E4" sqref="E4:E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.21875" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" customWidth="1"/>
+    <col min="5" max="5" width="30.08984375" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="8" max="9" width="13.6328125" customWidth="1"/>
+    <col min="10" max="10" width="17.6328125" customWidth="1"/>
+    <col min="11" max="11" width="16.08984375" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" customWidth="1"/>
+    <col min="14" max="14" width="16.08984375" customWidth="1"/>
+    <col min="15" max="15" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>117</v>
       </c>
@@ -966,7 +975,7 @@
       </c>
       <c r="N1" s="8"/>
     </row>
-    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1019,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -1021,12 +1030,12 @@
         <v>65</v>
       </c>
       <c r="D4" t="str">
-        <f>_xlfn.CONCAT(C4," ",B4)</f>
+        <f>PROPER(_xlfn.CONCAT(C4," ",B4))</f>
         <v>Stevie Bacata</v>
       </c>
       <c r="E4" t="str">
-        <f>C4&amp;"."&amp;B4&amp;"@pushpin.com"</f>
-        <v>Stevie.Bacata@pushpin.com</v>
+        <f>LOWER(C4&amp;"."&amp;B4&amp;"@pushpin.com")</f>
+        <v>stevie.bacata@pushpin.com</v>
       </c>
       <c r="F4" s="1">
         <v>39556</v>
@@ -1045,7 +1054,7 @@
       <c r="L4" s="1"/>
       <c r="M4" s="5"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1056,12 +1065,12 @@
         <v>17</v>
       </c>
       <c r="D5" t="str">
-        <f t="shared" ref="D5:D38" si="0">_xlfn.CONCAT(C5," ",B5)</f>
-        <v>Adam BARRY</v>
+        <f t="shared" ref="D5:D38" si="0">PROPER(_xlfn.CONCAT(C5," ",B5))</f>
+        <v>Adam Barry</v>
       </c>
       <c r="E5" t="str">
-        <f t="shared" ref="E5:E38" si="1">C5&amp;"."&amp;B5&amp;"@pushpin.com"</f>
-        <v>Adam.BARRY@pushpin.com</v>
+        <f t="shared" ref="E5:E38" si="1">LOWER(C5&amp;"."&amp;B5&amp;"@pushpin.com")</f>
+        <v>adam.barry@pushpin.com</v>
       </c>
       <c r="F5" s="1">
         <v>38104</v>
@@ -1080,7 +1089,7 @@
       <c r="L5" s="1"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -1096,7 +1105,7 @@
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>Connor.Betts@pushpin.com</v>
+        <v>connor.betts@pushpin.com</v>
       </c>
       <c r="F6" s="1">
         <v>41961</v>
@@ -1115,7 +1124,7 @@
       <c r="L6" s="1"/>
       <c r="M6" s="5"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -1127,7 +1136,7 @@
       </c>
       <c r="D7" t="str">
         <f t="shared" si="0"/>
-        <v>carlos martinez</v>
+        <v>Carlos Martinez</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
@@ -1150,7 +1159,7 @@
       <c r="L7" s="1"/>
       <c r="M7" s="5"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -1166,7 +1175,7 @@
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>Yvette.Biti@pushpin.com</v>
+        <v>yvette.biti@pushpin.com</v>
       </c>
       <c r="F8" s="1">
         <v>42389</v>
@@ -1185,7 +1194,7 @@
       <c r="L8" s="1"/>
       <c r="M8" s="5"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -1197,11 +1206,11 @@
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
-        <v>Jim BOLLER</v>
+        <v>Jim Boller</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>Jim.BOLLER@pushpin.com</v>
+        <v>jim.boller@pushpin.com</v>
       </c>
       <c r="F9" s="1">
         <v>41898</v>
@@ -1220,7 +1229,7 @@
       <c r="L9" s="1"/>
       <c r="M9" s="5"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -1236,7 +1245,7 @@
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>Charlie.Bui@pushpin.com</v>
+        <v>charlie.bui@pushpin.com</v>
       </c>
       <c r="F10" s="1">
         <v>41908</v>
@@ -1255,7 +1264,7 @@
       <c r="L10" s="1"/>
       <c r="M10" s="5"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -1271,7 +1280,7 @@
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>Tina.Carlton@pushpin.com</v>
+        <v>tina.carlton@pushpin.com</v>
       </c>
       <c r="F11" s="1">
         <v>38803</v>
@@ -1290,7 +1299,7 @@
       <c r="L11" s="1"/>
       <c r="M11" s="5"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1302,11 +1311,11 @@
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
-        <v>Joe CAROL</v>
+        <v>Joe Carol</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>Joe.CAROL@pushpin.com</v>
+        <v>joe.carol@pushpin.com</v>
       </c>
       <c r="F12" s="1">
         <v>36928</v>
@@ -1325,7 +1334,7 @@
       <c r="L12" s="1"/>
       <c r="M12" s="5"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>100</v>
       </c>
@@ -1337,11 +1346,11 @@
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
-        <v>Jim CHAFFEE</v>
+        <v>Jim Chaffee</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>Jim.CHAFFEE@pushpin.com</v>
+        <v>jim.chaffee@pushpin.com</v>
       </c>
       <c r="F13" s="1">
         <v>41792</v>
@@ -1360,7 +1369,7 @@
       <c r="L13" s="1"/>
       <c r="M13" s="5"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -1376,7 +1385,7 @@
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>Samantha.Chairs@pushpin.com</v>
+        <v>samantha.chairs@pushpin.com</v>
       </c>
       <c r="F14" s="1">
         <v>40595</v>
@@ -1395,7 +1404,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -1407,11 +1416,11 @@
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
-        <v>Uma CHAUDRI</v>
+        <v>Uma Chaudri</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
-        <v>Uma.CHAUDRI@pushpin.com</v>
+        <v>uma.chaudri@pushpin.com</v>
       </c>
       <c r="F15" s="1">
         <v>40994</v>
@@ -1430,7 +1439,7 @@
       <c r="L15" s="1"/>
       <c r="M15" s="5"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -1442,11 +1451,11 @@
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
-        <v>Elizabeth CHU</v>
+        <v>Elizabeth Chu</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>Elizabeth.CHU@pushpin.com</v>
+        <v>elizabeth.chu@pushpin.com</v>
       </c>
       <c r="F16" s="1">
         <v>40225</v>
@@ -1465,7 +1474,7 @@
       <c r="L16" s="1"/>
       <c r="M16" s="5"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1477,11 +1486,11 @@
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
-        <v>Eric CHUNG</v>
+        <v>Eric Chung</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
-        <v>Eric.CHUNG@pushpin.com</v>
+        <v>eric.chung@pushpin.com</v>
       </c>
       <c r="F17" s="1">
         <v>36955</v>
@@ -1500,7 +1509,7 @@
       <c r="L17" s="1"/>
       <c r="M17" s="5"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -1512,11 +1521,11 @@
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
-        <v>elizabeth CLARK</v>
+        <v>Elizabeth Clark</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>elizabeth.CLARK@pushpin.com</v>
+        <v>elizabeth.clark@pushpin.com</v>
       </c>
       <c r="F18" s="1">
         <v>42912</v>
@@ -1535,7 +1544,7 @@
       <c r="L18" s="1"/>
       <c r="M18" s="5"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -1547,11 +1556,11 @@
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
-        <v>ANNA CLARK</v>
+        <v>Anna Clark</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>ANNA.CLARK@pushpin.com</v>
+        <v>anna.clark@pushpin.com</v>
       </c>
       <c r="F19" s="1">
         <v>41995</v>
@@ -1570,7 +1579,7 @@
       <c r="L19" s="1"/>
       <c r="M19" s="5"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -1582,11 +1591,11 @@
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
-        <v>Sabrina COLE</v>
+        <v>Sabrina Cole</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>Sabrina.COLE@pushpin.com</v>
+        <v>sabrina.cole@pushpin.com</v>
       </c>
       <c r="F20" s="1">
         <v>41407</v>
@@ -1605,7 +1614,7 @@
       <c r="L20" s="1"/>
       <c r="M20" s="5"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -1617,11 +1626,11 @@
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
-        <v>Janet COMUNTZIS</v>
+        <v>Janet Comuntzis</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>Janet.COMUNTZIS@pushpin.com</v>
+        <v>janet.comuntzis@pushpin.com</v>
       </c>
       <c r="F21" s="1">
         <v>39692</v>
@@ -1640,7 +1649,7 @@
       <c r="L21" s="1"/>
       <c r="M21" s="5"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>98</v>
       </c>
@@ -1652,11 +1661,11 @@
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
-        <v>Bob DECKER</v>
+        <v>Bob Decker</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>Bob.DECKER@pushpin.com</v>
+        <v>bob.decker@pushpin.com</v>
       </c>
       <c r="F22" s="1">
         <v>41214</v>
@@ -1675,7 +1684,7 @@
       <c r="L22" s="1"/>
       <c r="M22" s="5"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -1687,11 +1696,11 @@
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
-        <v>Tina DESIATO</v>
+        <v>Tina Desiato</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
-        <v>Tina.DESIATO@pushpin.com</v>
+        <v>tina.desiato@pushpin.com</v>
       </c>
       <c r="F23" s="1">
         <v>41176</v>
@@ -1710,7 +1719,7 @@
       <c r="L23" s="1"/>
       <c r="M23" s="5"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>107</v>
       </c>
@@ -1722,11 +1731,11 @@
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
-        <v>Alexandra DONNELL</v>
+        <v>Alexandra Donnell</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
-        <v>Alexandra.DONNELL@pushpin.com</v>
+        <v>alexandra.donnell@pushpin.com</v>
       </c>
       <c r="F24" s="1">
         <v>42233</v>
@@ -1745,7 +1754,7 @@
       <c r="L24" s="1"/>
       <c r="M24" s="5"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -1757,11 +1766,11 @@
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
-        <v>Mark ELLIS</v>
+        <v>Mark Ellis</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="1"/>
-        <v>Mark.ELLIS@pushpin.com</v>
+        <v>mark.ellis@pushpin.com</v>
       </c>
       <c r="F25" s="1">
         <v>42376</v>
@@ -1780,7 +1789,7 @@
       <c r="L25" s="1"/>
       <c r="M25" s="5"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -1796,7 +1805,7 @@
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
-        <v>Nicholas.Fernandes@pushpin.com</v>
+        <v>nicholas.fernandes@pushpin.com</v>
       </c>
       <c r="F26" s="1">
         <v>39028</v>
@@ -1815,7 +1824,7 @@
       <c r="L26" s="1"/>
       <c r="M26" s="5"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -1827,11 +1836,11 @@
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
-        <v>Mary FERRIS</v>
+        <v>Mary Ferris</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="1"/>
-        <v>Mary.FERRIS@pushpin.com</v>
+        <v>mary.ferris@pushpin.com</v>
       </c>
       <c r="F27" s="1">
         <v>38553</v>
@@ -1850,7 +1859,7 @@
       <c r="L27" s="1"/>
       <c r="M27" s="5"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -1862,11 +1871,11 @@
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
-        <v>Susan FILOSA</v>
+        <v>Susan Filosa</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
-        <v>Susan.FILOSA@pushpin.com</v>
+        <v>susan.filosa@pushpin.com</v>
       </c>
       <c r="F28" s="1">
         <v>38749</v>
@@ -1885,7 +1894,7 @@
       <c r="L28" s="1"/>
       <c r="M28" s="5"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -1897,11 +1906,11 @@
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
-        <v>Daniel FLANDERS</v>
+        <v>Daniel Flanders</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
-        <v>Daniel.FLANDERS@pushpin.com</v>
+        <v>daniel.flanders@pushpin.com</v>
       </c>
       <c r="F29" s="1">
         <v>37515</v>
@@ -1920,7 +1929,7 @@
       <c r="L29" s="1"/>
       <c r="M29" s="5"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>106</v>
       </c>
@@ -1936,7 +1945,7 @@
       </c>
       <c r="E30" t="str">
         <f t="shared" si="1"/>
-        <v>Leighton.Forrest@pushpin.com</v>
+        <v>leighton.forrest@pushpin.com</v>
       </c>
       <c r="F30" s="1">
         <v>42125</v>
@@ -1955,7 +1964,7 @@
       <c r="L30" s="1"/>
       <c r="M30" s="5"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -1971,7 +1980,7 @@
       </c>
       <c r="E31" t="str">
         <f t="shared" si="1"/>
-        <v>Phoebe.Gour@pushpin.com</v>
+        <v>phoebe.gour@pushpin.com</v>
       </c>
       <c r="F31" s="1">
         <v>42726</v>
@@ -1990,7 +1999,7 @@
       <c r="L31" s="1"/>
       <c r="M31" s="5"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -2006,7 +2015,7 @@
       </c>
       <c r="E32" t="str">
         <f t="shared" si="1"/>
-        <v>Mihael.Khan@pushpin.com</v>
+        <v>mihael.khan@pushpin.com</v>
       </c>
       <c r="F32" s="1">
         <v>40162</v>
@@ -2025,7 +2034,7 @@
       <c r="L32" s="1"/>
       <c r="M32" s="5"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>113</v>
       </c>
@@ -2037,11 +2046,11 @@
       </c>
       <c r="D33" t="str">
         <f t="shared" si="0"/>
-        <v>Sean SANDERS</v>
+        <v>Sean Sanders</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="1"/>
-        <v>Sean.SANDERS@pushpin.com</v>
+        <v>sean.sanders@pushpin.com</v>
       </c>
       <c r="F33" s="1">
         <v>42892</v>
@@ -2060,7 +2069,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="5"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -2076,7 +2085,7 @@
       </c>
       <c r="E34" t="str">
         <f t="shared" si="1"/>
-        <v>Radhya.Staples@pushpin.com</v>
+        <v>radhya.staples@pushpin.com</v>
       </c>
       <c r="F34" s="1">
         <v>42325</v>
@@ -2095,7 +2104,7 @@
       <c r="L34" s="1"/>
       <c r="M34" s="5"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -2111,7 +2120,7 @@
       </c>
       <c r="E35" t="str">
         <f t="shared" si="1"/>
-        <v>Natasha.Song@pushpin.com</v>
+        <v>natasha.song@pushpin.com</v>
       </c>
       <c r="F35" s="1">
         <v>40714</v>
@@ -2130,7 +2139,7 @@
       <c r="L35" s="1"/>
       <c r="M35" s="5"/>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -2146,7 +2155,7 @@
       </c>
       <c r="E36" t="str">
         <f t="shared" si="1"/>
-        <v>Preston.Senome@pushpin.com</v>
+        <v>preston.senome@pushpin.com</v>
       </c>
       <c r="F36" s="1">
         <v>42326</v>
@@ -2165,7 +2174,7 @@
       <c r="L36" s="1"/>
       <c r="M36" s="5"/>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>115</v>
       </c>
@@ -2177,11 +2186,11 @@
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
-        <v>Mei WANG</v>
+        <v>Mei Wang</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="1"/>
-        <v>Mei.WANG@pushpin.com</v>
+        <v>mei.wang@pushpin.com</v>
       </c>
       <c r="F37" s="1">
         <v>40189</v>
@@ -2200,7 +2209,7 @@
       <c r="L37" s="1"/>
       <c r="M37" s="5"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>105</v>
       </c>
@@ -2216,7 +2225,7 @@
       </c>
       <c r="E38" t="str">
         <f t="shared" si="1"/>
-        <v>Aanya.Zhang@pushpin.com</v>
+        <v>aanya.zhang@pushpin.com</v>
       </c>
       <c r="F38" s="1">
         <v>42009</v>
@@ -2236,7 +2245,7 @@
       <c r="M38" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A4:M38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:M38">
     <sortCondition ref="B6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>